<commit_message>
update to manuscript and supplementary file indexing
</commit_message>
<xml_diff>
--- a/products/manuscript/supplementary_materials/Supplementary Data Table 5.xlsx
+++ b/products/manuscript/supplementary_materials/Supplementary Data Table 5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Desktop/GCMP/Supp_Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannah/Documents/OSUDocs/Projects/Disease_LHS/GCMP_Global_Disease/products/manuscript/supplementary_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86009FC0-6A4F-324A-BFFA-30DB9161D32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF17D8EF-941F-E848-8F3F-7165198625F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5540" yWindow="780" windowWidth="23260" windowHeight="12580" xr2:uid="{635964DC-1275-F24E-A533-4EEDB34ABDB9}"/>
   </bookViews>
@@ -189,7 +189,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">PGLS correlations between Endozoicomonas  relative abundance and host disease prevalence. </t>
+      <t xml:space="preserve">PGLS correlations between Endozoicomonas relative abundance and host disease prevalence. </t>
     </r>
     <r>
       <rPr>

</xml_diff>